<commit_message>
updated maps & maps panel
</commit_message>
<xml_diff>
--- a/data/fg500_2019_top10.xlsx
+++ b/data/fg500_2019_top10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahesh\github\fg500vsgdp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2668E2AF-8E6A-467F-A964-4C13AF0DED9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87727AC0-1033-4881-89C3-FCA1EAA4C5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="135" windowWidth="23925" windowHeight="15600" xr2:uid="{A1034A9A-1D25-4C07-85CF-FC2BB4648F04}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="23925" windowHeight="15600" xr2:uid="{A1034A9A-1D25-4C07-85CF-FC2BB4648F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>China National Petroleum</t>
   </si>
   <si>
-    <t>State Grid</t>
-  </si>
-  <si>
     <t>Saudi Aramco</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>Automobiles</t>
+  </si>
+  <si>
+    <t>State Grid (China)</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -496,19 +496,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3">
         <v>514</v>
@@ -539,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3">
         <v>415</v>
@@ -556,7 +556,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3">
         <v>397</v>
@@ -573,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3">
         <v>393</v>
@@ -584,13 +584,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3">
         <v>387</v>
@@ -601,13 +601,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3">
         <v>356</v>
@@ -618,13 +618,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3">
         <v>304</v>
@@ -635,13 +635,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3">
         <v>290</v>
@@ -652,13 +652,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3">
         <v>278</v>
@@ -669,13 +669,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3">
         <v>273</v>

</xml_diff>